<commit_message>
vormittag 28.02.2020: dokument verfeinern
</commit_message>
<xml_diff>
--- a/02_ZEITPLAN/zeitplan_28.02.2020_v02.xlsx
+++ b/02_ZEITPLAN/zeitplan_28.02.2020_v02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josiah\Documents\IPA2020_JOSIAH_SCHIESS\02_ZEITPLAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CB3AF68-0FE8-4F23-A058-92AED7E8AA44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E4F6BD-7355-4C4E-BC68-739D1E84DDAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{74D2615D-1CED-415F-A807-8E49B652F1F1}"/>
+    <workbookView xWindow="-25320" yWindow="435" windowWidth="25440" windowHeight="15990" xr2:uid="{74D2615D-1CED-415F-A807-8E49B652F1F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan final" sheetId="2" r:id="rId1"/>
@@ -688,18 +688,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,6 +703,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -724,19 +721,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4092,9 +4092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47C3C77-DD25-4E69-9FF0-12031AADE1AE}">
   <dimension ref="A1:AX81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S57" sqref="S57"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,245 +4150,245 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37" t="s">
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37" t="s">
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37" t="s">
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37" t="s">
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37" t="s">
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37" t="s">
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37" t="s">
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="50"/>
+      <c r="AR1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
     </row>
     <row r="2" spans="1:50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37" t="s">
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37" t="s">
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37" t="s">
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37" t="s">
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37" t="s">
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37" t="s">
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37" t="s">
+      <c r="AG2" s="50"/>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37" t="s">
+      <c r="AK2" s="50"/>
+      <c r="AL2" s="50"/>
+      <c r="AM2" s="50"/>
+      <c r="AN2" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37" t="s">
+      <c r="AO2" s="50"/>
+      <c r="AP2" s="50"/>
+      <c r="AQ2" s="50"/>
+      <c r="AR2" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
+      <c r="AS2" s="50"/>
+      <c r="AT2" s="50"/>
+      <c r="AU2" s="50"/>
     </row>
     <row r="3" spans="1:50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="39" t="s">
+      <c r="E3" s="50"/>
+      <c r="F3" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="50"/>
+      <c r="J3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37" t="s">
+      <c r="S3" s="50"/>
+      <c r="T3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37" t="s">
+      <c r="U3" s="50"/>
+      <c r="V3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37" t="s">
+      <c r="W3" s="50"/>
+      <c r="X3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37" t="s">
+      <c r="Y3" s="50"/>
+      <c r="Z3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37" t="s">
+      <c r="AA3" s="50"/>
+      <c r="AB3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37" t="s">
+      <c r="AC3" s="50"/>
+      <c r="AD3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37" t="s">
+      <c r="AE3" s="50"/>
+      <c r="AF3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37" t="s">
+      <c r="AG3" s="50"/>
+      <c r="AH3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37" t="s">
+      <c r="AI3" s="50"/>
+      <c r="AJ3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37" t="s">
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37" t="s">
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="37" t="s">
+      <c r="AO3" s="50"/>
+      <c r="AP3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AQ3" s="37"/>
-      <c r="AR3" s="37" t="s">
+      <c r="AQ3" s="50"/>
+      <c r="AR3" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AS3" s="37"/>
-      <c r="AT3" s="37" t="s">
+      <c r="AS3" s="50"/>
+      <c r="AT3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AU3" s="37"/>
+      <c r="AU3" s="50"/>
     </row>
     <row r="4" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -4442,16 +4442,16 @@
       <c r="AU4" s="1"/>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B5" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>11</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="38">
         <f>SUM(D6:AU6)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -4521,9 +4521,9 @@
       </c>
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="11"/>
       <c r="E6" s="28"/>
       <c r="F6" s="11"/>
@@ -4586,18 +4586,20 @@
       </c>
       <c r="AR6" s="11"/>
       <c r="AS6" s="11"/>
-      <c r="AT6" s="11"/>
+      <c r="AT6" s="11">
+        <v>1</v>
+      </c>
       <c r="AU6" s="11"/>
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B7" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C7" s="42">
+      <c r="C7" s="38">
         <f>SUM(D8:AU8)</f>
         <v>4</v>
       </c>
@@ -4653,9 +4655,9 @@
       <c r="AU7" s="11"/>
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="11">
         <v>1</v>
       </c>
@@ -4714,14 +4716,14 @@
       <c r="AX8" s="49"/>
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B9" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>2</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="38">
         <f>SUM(D10:AU10)</f>
         <v>3</v>
       </c>
@@ -4779,9 +4781,9 @@
       </c>
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -4836,14 +4838,14 @@
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="42">
+      <c r="B11" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>5</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="38">
         <f>SUM(D12:AU12)</f>
         <v>0</v>
       </c>
@@ -4903,9 +4905,9 @@
       </c>
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="A12" s="37"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -5068,14 +5070,14 @@
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="42">
+      <c r="B15" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>2</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="38">
         <f>SUM(D16:AU16)</f>
         <v>3</v>
       </c>
@@ -5131,9 +5133,9 @@
       </c>
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="11">
         <v>2</v>
       </c>
@@ -5184,14 +5186,14 @@
       <c r="AU16" s="11"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="38">
         <f>SUM(D18:AU18)</f>
         <v>1</v>
       </c>
@@ -5249,9 +5251,9 @@
       </c>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
+      <c r="A18" s="37"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="11"/>
       <c r="E18" s="13">
         <v>1</v>
@@ -5306,14 +5308,14 @@
       </c>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="42">
+      <c r="B19" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="38">
         <f>SUM(D20:AU20)</f>
         <v>1</v>
       </c>
@@ -5371,9 +5373,9 @@
       </c>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11">
@@ -5428,14 +5430,14 @@
       </c>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="38">
         <f>SUM(D22:AU22)</f>
         <v>1</v>
       </c>
@@ -5493,9 +5495,9 @@
       </c>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11">
@@ -5550,14 +5552,14 @@
       </c>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="42">
+      <c r="B23" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="38">
         <f>SUM(D24:AU24)</f>
         <v>1</v>
       </c>
@@ -5615,9 +5617,9 @@
       </c>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -5666,14 +5668,14 @@
       <c r="AU24" s="11"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="38">
         <f>SUM(D26:AU26)</f>
         <v>1</v>
       </c>
@@ -5725,9 +5727,9 @@
       <c r="AU25" s="11"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -5776,16 +5778,16 @@
       <c r="AU26" s="11"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="42">
+      <c r="B27" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="38">
         <f>SUM(D28:AU28)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -5835,9 +5837,9 @@
       <c r="AU27" s="11"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -5880,7 +5882,9 @@
       <c r="AQ28" s="11"/>
       <c r="AR28" s="11"/>
       <c r="AS28" s="11"/>
-      <c r="AT28" s="11"/>
+      <c r="AT28" s="11">
+        <v>1</v>
+      </c>
       <c r="AU28" s="11"/>
     </row>
     <row r="29" spans="1:50" ht="15.75" x14ac:dyDescent="0.25">
@@ -6084,14 +6088,14 @@
       <c r="AU32" s="11"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="42">
+      <c r="B33" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="38">
         <f>SUM(D34:AU34)</f>
         <v>1</v>
       </c>
@@ -6143,9 +6147,9 @@
       <c r="AU33" s="11"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -6194,14 +6198,14 @@
       <c r="AU34" s="11"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="42">
+      <c r="B35" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>2</v>
       </c>
-      <c r="C35" s="42">
+      <c r="C35" s="38">
         <f>SUM(D36:AU36)</f>
         <v>1</v>
       </c>
@@ -6253,9 +6257,9 @@
       <c r="AU35" s="11"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -6304,14 +6308,14 @@
       <c r="AU36" s="11"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="42">
+      <c r="B37" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C37" s="42">
+      <c r="C37" s="38">
         <f>SUM(D38:AU38)</f>
         <v>1</v>
       </c>
@@ -6363,9 +6367,9 @@
       <c r="AU37" s="11"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -6514,14 +6518,14 @@
       <c r="AU40" s="12"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="42">
+      <c r="B41" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C41" s="42">
+      <c r="C41" s="38">
         <f>SUM(D42:AU42)</f>
         <v>1</v>
       </c>
@@ -6573,9 +6577,9 @@
       <c r="AU41" s="11"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -6624,14 +6628,14 @@
       <c r="AU42" s="11"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="42">
+      <c r="B43" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C43" s="42">
+      <c r="C43" s="38">
         <f>SUM(D44:AU44)</f>
         <v>3</v>
       </c>
@@ -6685,9 +6689,9 @@
       <c r="AU43" s="11"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A44" s="41"/>
-      <c r="B44" s="42"/>
-      <c r="C44" s="42"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
@@ -6738,14 +6742,14 @@
       <c r="AU44" s="11"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="42">
+      <c r="B45" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C45" s="42">
+      <c r="C45" s="38">
         <f>SUM(D46:AU46)</f>
         <v>3</v>
       </c>
@@ -6799,9 +6803,9 @@
       <c r="AU45" s="11"/>
     </row>
     <row r="46" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A46" s="41"/>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
@@ -6852,14 +6856,14 @@
       <c r="AU46" s="11"/>
     </row>
     <row r="47" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C47" s="42">
+      <c r="C47" s="38">
         <f>SUM(D48:AU48)</f>
         <v>3</v>
       </c>
@@ -6913,9 +6917,9 @@
       <c r="AU47" s="11"/>
     </row>
     <row r="48" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A48" s="41"/>
-      <c r="B48" s="42"/>
-      <c r="C48" s="42"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="38"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -6966,14 +6970,14 @@
       <c r="AU48" s="11"/>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="42">
+      <c r="B49" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>4</v>
       </c>
-      <c r="C49" s="42">
+      <c r="C49" s="38">
         <f>SUM(D50:AU50)</f>
         <v>5</v>
       </c>
@@ -7029,9 +7033,9 @@
       <c r="AU49" s="11"/>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A50" s="41"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
+      <c r="C50" s="38"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -7184,14 +7188,14 @@
       <c r="AU52" s="14"/>
     </row>
     <row r="53" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B53" s="42">
+      <c r="B53" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C53" s="42">
+      <c r="C53" s="38">
         <f>SUM(D54:AU54)</f>
         <v>1</v>
       </c>
@@ -7243,9 +7247,9 @@
       <c r="AU53" s="11"/>
     </row>
     <row r="54" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A54" s="41"/>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
@@ -7294,14 +7298,14 @@
       <c r="AU54" s="11"/>
     </row>
     <row r="55" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="42">
+      <c r="B55" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>4</v>
       </c>
-      <c r="C55" s="42">
+      <c r="C55" s="38">
         <f>SUM(D56:AU56)</f>
         <v>4</v>
       </c>
@@ -7357,9 +7361,9 @@
       <c r="AU55" s="11"/>
     </row>
     <row r="56" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
-      <c r="B56" s="42"/>
-      <c r="C56" s="42"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -7410,14 +7414,14 @@
       <c r="AU56" s="11"/>
     </row>
     <row r="57" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B57" s="42">
+      <c r="B57" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C57" s="42">
+      <c r="C57" s="38">
         <f>SUM(D58:AU58)</f>
         <v>2</v>
       </c>
@@ -7473,9 +7477,9 @@
       <c r="AU57" s="11"/>
     </row>
     <row r="58" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A58" s="41"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="38"/>
+      <c r="C58" s="38"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -7526,14 +7530,14 @@
       <c r="AU58" s="11"/>
     </row>
     <row r="59" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B59" s="42">
+      <c r="B59" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>2</v>
       </c>
-      <c r="C59" s="42">
+      <c r="C59" s="38">
         <f>SUM(D60:AU60)</f>
         <v>2</v>
       </c>
@@ -7587,9 +7591,9 @@
       <c r="AU59" s="11"/>
     </row>
     <row r="60" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A60" s="41"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="38"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -7640,14 +7644,14 @@
       <c r="AU60" s="11"/>
     </row>
     <row r="61" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A61" s="41" t="s">
+      <c r="A61" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B61" s="42">
+      <c r="B61" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>1</v>
       </c>
-      <c r="C61" s="42">
+      <c r="C61" s="38">
         <f>SUM(D62:AU62)</f>
         <v>1</v>
       </c>
@@ -7699,9 +7703,9 @@
       <c r="AU61" s="11"/>
     </row>
     <row r="62" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A62" s="41"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="42"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="38"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -7750,14 +7754,14 @@
       <c r="AU62" s="11"/>
     </row>
     <row r="63" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="B63" s="42">
+      <c r="B63" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C63" s="42">
+      <c r="C63" s="38">
         <f>SUM(D64:AU64)</f>
         <v>4</v>
       </c>
@@ -7814,9 +7818,9 @@
       <c r="AX63" s="10"/>
     </row>
     <row r="64" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A64" s="41"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="42"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -7869,14 +7873,14 @@
       <c r="AU64" s="11"/>
     </row>
     <row r="65" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
+      <c r="A65" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="42">
+      <c r="B65" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>4</v>
       </c>
-      <c r="C65" s="42">
+      <c r="C65" s="38">
         <f>SUM(D66:AU66)</f>
         <v>4</v>
       </c>
@@ -7935,9 +7939,9 @@
       <c r="AX65" s="10"/>
     </row>
     <row r="66" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
-      <c r="B66" s="42"/>
-      <c r="C66" s="42"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -7988,14 +7992,14 @@
       <c r="AU66" s="11"/>
     </row>
     <row r="67" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="B67" s="42">
+      <c r="B67" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>4</v>
       </c>
-      <c r="C67" s="42">
+      <c r="C67" s="38">
         <f>SUM(D68:AU68)</f>
         <v>3</v>
       </c>
@@ -8051,9 +8055,9 @@
       <c r="AU67" s="11"/>
     </row>
     <row r="68" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A68" s="41"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="42"/>
+      <c r="A68" s="37"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -8104,14 +8108,14 @@
       <c r="AU68" s="11"/>
     </row>
     <row r="69" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A69" s="41" t="s">
+      <c r="A69" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="42">
+      <c r="B69" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>4</v>
       </c>
-      <c r="C69" s="42">
+      <c r="C69" s="38">
         <f>SUM(D70:AU70)</f>
         <v>3</v>
       </c>
@@ -8167,9 +8171,9 @@
       <c r="AU69" s="11"/>
     </row>
     <row r="70" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A70" s="41"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
+      <c r="A70" s="37"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -8220,14 +8224,14 @@
       <c r="AU70" s="11"/>
     </row>
     <row r="71" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A71" s="41" t="s">
+      <c r="A71" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="42">
+      <c r="B71" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>3</v>
       </c>
-      <c r="C71" s="42">
+      <c r="C71" s="38">
         <f>SUM(D72:AU72)</f>
         <v>1</v>
       </c>
@@ -8281,9 +8285,9 @@
       <c r="AU71" s="11"/>
     </row>
     <row r="72" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A72" s="41"/>
-      <c r="B72" s="42"/>
-      <c r="C72" s="42"/>
+      <c r="A72" s="37"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="38"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -8432,16 +8436,16 @@
       <c r="AU74" s="12"/>
     </row>
     <row r="75" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="42">
+      <c r="B75" s="38">
         <f>SUM(Table24[#This Row])</f>
         <v>5</v>
       </c>
-      <c r="C75" s="42">
+      <c r="C75" s="38">
         <f>SUM(D76:AU76)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
@@ -8495,9 +8499,9 @@
       <c r="AU75" s="11"/>
     </row>
     <row r="76" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A76" s="41"/>
-      <c r="B76" s="42"/>
-      <c r="C76" s="42"/>
+      <c r="A76" s="37"/>
+      <c r="B76" s="38"/>
+      <c r="C76" s="38"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
@@ -8546,10 +8550,16 @@
       <c r="AQ76" s="11">
         <v>1</v>
       </c>
-      <c r="AR76" s="11"/>
-      <c r="AS76" s="11"/>
+      <c r="AR76" s="11">
+        <v>2</v>
+      </c>
+      <c r="AS76" s="11">
+        <v>2</v>
+      </c>
       <c r="AT76" s="11"/>
-      <c r="AU76" s="11"/>
+      <c r="AU76" s="11">
+        <v>2</v>
+      </c>
     </row>
     <row r="77" spans="1:50" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
@@ -8692,7 +8702,7 @@
       </c>
       <c r="C78" s="25">
         <f>SUM(C5:C76)</f>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="D78" s="15" cm="1">
         <f t="array" ref="D78">SUM(IF(MOD(1+ ROW( Table24[[#All],[Column1]:[Column4]]),2)=0,Table24[[#All],[Column1]:[Column4]],0))</f>
@@ -8848,7 +8858,7 @@
       </c>
       <c r="AS78" s="16" cm="1">
         <f t="array" ref="AS78">SUM(IF(MOD(ROW(Table24[[#All],[Column2]:[Column3]]),2)=0,Table24[[#All],[Column2]:[Column3]],0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT78" s="16" cm="1">
         <f t="array" ref="AT78">SUM(IF(MOD(1+ ROW(Table24[[#All],[Column6]:[Column7]]),2)=0,Table24[[#All],[Column6]:[Column7]],0))</f>
@@ -8856,255 +8866,412 @@
       </c>
       <c r="AU78" s="16" cm="1">
         <f t="array" ref="AU78">SUM(IF(MOD(ROW(Table24[[#All],[Column6]:[Column7]]),2)=0,Table24[[#All],[Column6]:[Column7]],0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AV78" s="3"/>
       <c r="AW78" s="3"/>
       <c r="AX78" s="3"/>
     </row>
     <row r="79" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A79" s="53" t="s">
+      <c r="A79" s="48" t="s">
         <v>29</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="17"/>
-      <c r="D79" s="46" t="s">
+      <c r="D79" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="E79" s="47"/>
-      <c r="F79" s="47"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I79" s="47"/>
-      <c r="J79" s="47"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="46" t="s">
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="I79" s="46"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="M79" s="47"/>
-      <c r="N79" s="47"/>
-      <c r="O79" s="48"/>
-      <c r="P79" s="46" t="s">
+      <c r="M79" s="46"/>
+      <c r="N79" s="46"/>
+      <c r="O79" s="47"/>
+      <c r="P79" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="Q79" s="47"/>
-      <c r="R79" s="47"/>
-      <c r="S79" s="48"/>
-      <c r="T79" s="46" t="s">
+      <c r="Q79" s="46"/>
+      <c r="R79" s="46"/>
+      <c r="S79" s="47"/>
+      <c r="T79" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="U79" s="47"/>
-      <c r="V79" s="47"/>
-      <c r="W79" s="48"/>
-      <c r="X79" s="46" t="s">
+      <c r="U79" s="46"/>
+      <c r="V79" s="46"/>
+      <c r="W79" s="47"/>
+      <c r="X79" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="Y79" s="47"/>
-      <c r="Z79" s="47"/>
-      <c r="AA79" s="48"/>
-      <c r="AB79" s="46" t="s">
+      <c r="Y79" s="46"/>
+      <c r="Z79" s="46"/>
+      <c r="AA79" s="47"/>
+      <c r="AB79" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="AC79" s="47"/>
-      <c r="AD79" s="47"/>
-      <c r="AE79" s="48"/>
-      <c r="AF79" s="46" t="s">
+      <c r="AC79" s="46"/>
+      <c r="AD79" s="46"/>
+      <c r="AE79" s="47"/>
+      <c r="AF79" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="AG79" s="47"/>
-      <c r="AH79" s="47"/>
-      <c r="AI79" s="48"/>
-      <c r="AJ79" s="46" t="s">
+      <c r="AG79" s="46"/>
+      <c r="AH79" s="46"/>
+      <c r="AI79" s="47"/>
+      <c r="AJ79" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="AK79" s="47"/>
-      <c r="AL79" s="47"/>
-      <c r="AM79" s="48"/>
-      <c r="AN79" s="46" t="s">
+      <c r="AK79" s="46"/>
+      <c r="AL79" s="46"/>
+      <c r="AM79" s="47"/>
+      <c r="AN79" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="AO79" s="47"/>
-      <c r="AP79" s="47"/>
-      <c r="AQ79" s="48"/>
-      <c r="AR79" s="46" t="s">
+      <c r="AO79" s="46"/>
+      <c r="AP79" s="46"/>
+      <c r="AQ79" s="47"/>
+      <c r="AR79" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="AS79" s="47"/>
-      <c r="AT79" s="47"/>
-      <c r="AU79" s="48"/>
+      <c r="AS79" s="46"/>
+      <c r="AT79" s="46"/>
+      <c r="AU79" s="47"/>
     </row>
     <row r="80" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A80" s="53"/>
+      <c r="A80" s="48"/>
       <c r="B80" s="26"/>
       <c r="C80" s="17"/>
-      <c r="D80" s="43" t="s">
+      <c r="D80" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="45"/>
-      <c r="H80" s="43" t="s">
+      <c r="E80" s="40"/>
+      <c r="F80" s="40"/>
+      <c r="G80" s="41"/>
+      <c r="H80" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="45"/>
-      <c r="L80" s="43" t="s">
+      <c r="I80" s="40"/>
+      <c r="J80" s="40"/>
+      <c r="K80" s="41"/>
+      <c r="L80" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
-      <c r="O80" s="45"/>
-      <c r="P80" s="43" t="s">
+      <c r="M80" s="40"/>
+      <c r="N80" s="40"/>
+      <c r="O80" s="41"/>
+      <c r="P80" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="Q80" s="44"/>
-      <c r="R80" s="44"/>
-      <c r="S80" s="45"/>
-      <c r="T80" s="43" t="s">
+      <c r="Q80" s="40"/>
+      <c r="R80" s="40"/>
+      <c r="S80" s="41"/>
+      <c r="T80" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="U80" s="44"/>
-      <c r="V80" s="44"/>
-      <c r="W80" s="45"/>
-      <c r="X80" s="43" t="s">
+      <c r="U80" s="40"/>
+      <c r="V80" s="40"/>
+      <c r="W80" s="41"/>
+      <c r="X80" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="Y80" s="44"/>
-      <c r="Z80" s="44"/>
-      <c r="AA80" s="45"/>
-      <c r="AB80" s="43" t="s">
+      <c r="Y80" s="40"/>
+      <c r="Z80" s="40"/>
+      <c r="AA80" s="41"/>
+      <c r="AB80" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="AC80" s="44"/>
-      <c r="AD80" s="44"/>
-      <c r="AE80" s="45"/>
-      <c r="AF80" s="43" t="s">
+      <c r="AC80" s="40"/>
+      <c r="AD80" s="40"/>
+      <c r="AE80" s="41"/>
+      <c r="AF80" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="AG80" s="44"/>
-      <c r="AH80" s="44"/>
-      <c r="AI80" s="45"/>
-      <c r="AJ80" s="43" t="s">
+      <c r="AG80" s="40"/>
+      <c r="AH80" s="40"/>
+      <c r="AI80" s="41"/>
+      <c r="AJ80" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="AK80" s="44"/>
-      <c r="AL80" s="44"/>
-      <c r="AM80" s="45"/>
-      <c r="AN80" s="43" t="s">
+      <c r="AK80" s="40"/>
+      <c r="AL80" s="40"/>
+      <c r="AM80" s="41"/>
+      <c r="AN80" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="AO80" s="44"/>
-      <c r="AP80" s="44"/>
-      <c r="AQ80" s="45"/>
-      <c r="AR80" s="43" t="s">
+      <c r="AO80" s="40"/>
+      <c r="AP80" s="40"/>
+      <c r="AQ80" s="41"/>
+      <c r="AR80" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="AS80" s="44"/>
-      <c r="AT80" s="44"/>
-      <c r="AU80" s="45"/>
+      <c r="AS80" s="40"/>
+      <c r="AT80" s="40"/>
+      <c r="AU80" s="41"/>
     </row>
     <row r="81" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A81" s="53"/>
+      <c r="A81" s="48"/>
       <c r="B81" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="50" t="s">
+      <c r="D81" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E81" s="51"/>
-      <c r="F81" s="51" t="s">
+      <c r="E81" s="43"/>
+      <c r="F81" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="G81" s="52"/>
-      <c r="H81" s="43" t="s">
+      <c r="G81" s="44"/>
+      <c r="H81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="I81" s="44"/>
-      <c r="J81" s="44" t="s">
+      <c r="I81" s="40"/>
+      <c r="J81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="K81" s="45"/>
-      <c r="L81" s="43" t="s">
+      <c r="K81" s="41"/>
+      <c r="L81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="M81" s="44"/>
-      <c r="N81" s="44" t="s">
+      <c r="M81" s="40"/>
+      <c r="N81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="O81" s="44"/>
-      <c r="P81" s="43" t="s">
+      <c r="O81" s="40"/>
+      <c r="P81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Q81" s="44"/>
-      <c r="R81" s="44" t="s">
+      <c r="Q81" s="40"/>
+      <c r="R81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="S81" s="45"/>
-      <c r="T81" s="43" t="s">
+      <c r="S81" s="41"/>
+      <c r="T81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="U81" s="44"/>
-      <c r="V81" s="44" t="s">
+      <c r="U81" s="40"/>
+      <c r="V81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="W81" s="45"/>
-      <c r="X81" s="43" t="s">
+      <c r="W81" s="41"/>
+      <c r="X81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="Y81" s="44"/>
-      <c r="Z81" s="44" t="s">
+      <c r="Y81" s="40"/>
+      <c r="Z81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AA81" s="45"/>
-      <c r="AB81" s="43" t="s">
+      <c r="AA81" s="41"/>
+      <c r="AB81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AC81" s="44"/>
-      <c r="AD81" s="44" t="s">
+      <c r="AC81" s="40"/>
+      <c r="AD81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AE81" s="45"/>
-      <c r="AF81" s="43" t="s">
+      <c r="AE81" s="41"/>
+      <c r="AF81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AG81" s="44"/>
-      <c r="AH81" s="44" t="s">
+      <c r="AG81" s="40"/>
+      <c r="AH81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AI81" s="45"/>
-      <c r="AJ81" s="44" t="s">
+      <c r="AI81" s="41"/>
+      <c r="AJ81" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="AK81" s="44"/>
-      <c r="AL81" s="44" t="s">
+      <c r="AK81" s="40"/>
+      <c r="AL81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AM81" s="45"/>
-      <c r="AN81" s="43" t="s">
+      <c r="AM81" s="41"/>
+      <c r="AN81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AO81" s="44"/>
-      <c r="AP81" s="44" t="s">
+      <c r="AO81" s="40"/>
+      <c r="AP81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AQ81" s="45"/>
-      <c r="AR81" s="43" t="s">
+      <c r="AQ81" s="41"/>
+      <c r="AR81" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="AS81" s="44"/>
-      <c r="AT81" s="44" t="s">
+      <c r="AS81" s="40"/>
+      <c r="AT81" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AU81" s="45"/>
+      <c r="AU81" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="181">
+    <mergeCell ref="X1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AN1:AQ1"/>
+    <mergeCell ref="AR1:AU1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="AF2:AI2"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN2:AQ2"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D80:G80"/>
+    <mergeCell ref="H80:K80"/>
+    <mergeCell ref="L80:O80"/>
+    <mergeCell ref="AB80:AE80"/>
+    <mergeCell ref="L79:O79"/>
+    <mergeCell ref="P79:S79"/>
+    <mergeCell ref="T79:W79"/>
+    <mergeCell ref="X79:AA79"/>
+    <mergeCell ref="AB79:AE79"/>
+    <mergeCell ref="AT81:AU81"/>
+    <mergeCell ref="AW8:AX8"/>
+    <mergeCell ref="AB81:AC81"/>
+    <mergeCell ref="AD81:AE81"/>
+    <mergeCell ref="AF81:AG81"/>
+    <mergeCell ref="AH81:AI81"/>
+    <mergeCell ref="AJ81:AK81"/>
+    <mergeCell ref="AL81:AM81"/>
+    <mergeCell ref="P81:Q81"/>
+    <mergeCell ref="R81:S81"/>
+    <mergeCell ref="T81:U81"/>
+    <mergeCell ref="V81:W81"/>
+    <mergeCell ref="X81:Y81"/>
+    <mergeCell ref="Z81:AA81"/>
+    <mergeCell ref="AF80:AI80"/>
+    <mergeCell ref="AJ80:AM80"/>
+    <mergeCell ref="AN80:AQ80"/>
+    <mergeCell ref="AR80:AU80"/>
+    <mergeCell ref="AJ79:AM79"/>
+    <mergeCell ref="AN79:AQ79"/>
+    <mergeCell ref="AR79:AU79"/>
+    <mergeCell ref="P80:S80"/>
+    <mergeCell ref="T80:W80"/>
+    <mergeCell ref="X80:AA80"/>
     <mergeCell ref="A69:A70"/>
     <mergeCell ref="B69:B70"/>
     <mergeCell ref="C69:C70"/>
@@ -9129,163 +9296,6 @@
     <mergeCell ref="H79:K79"/>
     <mergeCell ref="A71:A72"/>
     <mergeCell ref="B71:B72"/>
-    <mergeCell ref="AT81:AU81"/>
-    <mergeCell ref="AW8:AX8"/>
-    <mergeCell ref="AB81:AC81"/>
-    <mergeCell ref="AD81:AE81"/>
-    <mergeCell ref="AF81:AG81"/>
-    <mergeCell ref="AH81:AI81"/>
-    <mergeCell ref="AJ81:AK81"/>
-    <mergeCell ref="AL81:AM81"/>
-    <mergeCell ref="P81:Q81"/>
-    <mergeCell ref="R81:S81"/>
-    <mergeCell ref="T81:U81"/>
-    <mergeCell ref="V81:W81"/>
-    <mergeCell ref="X81:Y81"/>
-    <mergeCell ref="Z81:AA81"/>
-    <mergeCell ref="AF80:AI80"/>
-    <mergeCell ref="AJ80:AM80"/>
-    <mergeCell ref="AN80:AQ80"/>
-    <mergeCell ref="AR80:AU80"/>
-    <mergeCell ref="AJ79:AM79"/>
-    <mergeCell ref="AN79:AQ79"/>
-    <mergeCell ref="AR79:AU79"/>
-    <mergeCell ref="P80:S80"/>
-    <mergeCell ref="T80:W80"/>
-    <mergeCell ref="X80:AA80"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D80:G80"/>
-    <mergeCell ref="H80:K80"/>
-    <mergeCell ref="L80:O80"/>
-    <mergeCell ref="AB80:AE80"/>
-    <mergeCell ref="L79:O79"/>
-    <mergeCell ref="P79:S79"/>
-    <mergeCell ref="T79:W79"/>
-    <mergeCell ref="X79:AA79"/>
-    <mergeCell ref="AB79:AE79"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="AF2:AI2"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN2:AQ2"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AN1:AQ1"/>
-    <mergeCell ref="AR1:AU1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:W1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="L2:O2"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:AU20 D65:AU68 D71:AU76 D61:AU62 D25:AU58">
     <cfRule type="expression" dxfId="148" priority="13">

</xml_diff>